<commit_message>
Fully finished and tested userstory 30 and 31
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,15 +462,20 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>alive</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>age</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>spouse</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>death</t>
         </is>
@@ -505,11 +510,14 @@
           <t>F1</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
         <v>23</v>
       </c>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -540,15 +548,18 @@
           <t>F3</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
         <v>53</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>F2</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -579,15 +590,18 @@
           <t>F4</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
         <v>52</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>F1</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -618,11 +632,14 @@
           <t>F1</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
         <v>23</v>
       </c>
-      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -649,15 +666,18 @@
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
         <v>78</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>F4</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -684,15 +704,18 @@
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
         <v>77</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>F4</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -719,15 +742,18 @@
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
         <v>32</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>F2</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -754,11 +780,14 @@
           <t>F2</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
         <v>5</v>
       </c>
-      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -785,15 +814,18 @@
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
         <v>66</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>F5</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t xml:space="preserve"> 5 JUN 2010</t>
         </is>
@@ -824,15 +856,18 @@
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="n">
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
         <v>36</v>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>F3</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t xml:space="preserve"> 5 MAY 1980</t>
         </is>
@@ -863,15 +898,18 @@
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="n">
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
         <v>59</v>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>F5</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t xml:space="preserve"> 9 AUG 2009</t>
         </is>
@@ -888,7 +926,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -937,6 +975,11 @@
           <t>divorced</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>are divorced</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -982,6 +1025,7 @@
           <t xml:space="preserve"> 10 JUL 2015</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1023,6 +1067,7 @@
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1064,6 +1109,7 @@
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1105,6 +1151,9 @@
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1142,6 +1191,7 @@
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added more acceptance tests (need to fix line number)
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,40 +442,45 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>gender</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>birthday</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>child</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>alive</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>age</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>spouse</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>death</t>
         </is>
@@ -490,34 +495,37 @@
           <t>I1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Tom /Brindley/</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t xml:space="preserve"> 20 JUL 1999</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>F1</t>
         </is>
       </c>
-      <c r="G2" t="b">
+      <c r="H2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>23</v>
       </c>
-      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -528,38 +536,41 @@
           <t>I2</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>24</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t xml:space="preserve"> Steven /Brindley/</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2 JUL 1969</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>F3</t>
         </is>
       </c>
-      <c r="G3" t="b">
+      <c r="H3" t="b">
         <v>1</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>53</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>F2</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>['F1', 'F2']</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -570,38 +581,41 @@
           <t>I3</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>35</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t xml:space="preserve"> Amy /Brooks/</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t xml:space="preserve"> 4 APR 1970</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>F4</t>
         </is>
       </c>
-      <c r="G4" t="b">
+      <c r="H4" t="b">
         <v>1</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>52</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>F1</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>['F1']</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -612,34 +626,37 @@
           <t>I4</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>44</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t xml:space="preserve"> Sophia /Brindley/</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t xml:space="preserve"> 20 JUL 1999</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>F1</t>
         </is>
       </c>
-      <c r="G5" t="b">
+      <c r="H5" t="b">
         <v>1</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>23</v>
       </c>
-      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -650,34 +667,37 @@
           <t>I5</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>53</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t xml:space="preserve"> Erin /Brooks/</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 6 JUN 1944</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="b">
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="b">
         <v>1</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>78</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>F4</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>['F4']</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -688,34 +708,37 @@
           <t>I6</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>62</v>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t xml:space="preserve"> Josie /Campbell/</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t xml:space="preserve"> 5 JUN 1945</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="b">
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="b">
         <v>1</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>77</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>F4</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>['F4']</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -726,34 +749,37 @@
           <t>I7</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>71</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t xml:space="preserve"> Lisa /Rutherford/</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t xml:space="preserve"> 5 MAR 1990</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="b">
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="b">
         <v>1</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>32</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>F2</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>['F2']</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -764,30 +790,33 @@
           <t>I8</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>80</v>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t xml:space="preserve"> Reginald /Brindley/</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
         <is>
           <t xml:space="preserve"> 10 AUG 2017</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>F2</t>
         </is>
       </c>
-      <c r="G9" t="b">
+      <c r="H9" t="b">
         <v>1</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>5</v>
       </c>
-      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -798,34 +827,37 @@
           <t>I9</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" t="n">
+        <v>88</v>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t xml:space="preserve"> Tim /Brindley/</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t xml:space="preserve"> 4 MAY 1944</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="b">
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="b">
         <v>0</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>66</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>F5</t>
-        </is>
-      </c>
       <c r="J10" t="inlineStr">
+        <is>
+          <t>['F3', 'F5']</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t xml:space="preserve"> 5 JUN 2010</t>
         </is>
@@ -840,34 +872,37 @@
           <t>I10</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t xml:space="preserve"> Selina /Rosemary/</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t xml:space="preserve"> 5 APR 1944</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="b">
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="b">
         <v>0</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>36</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>F3</t>
-        </is>
-      </c>
       <c r="J11" t="inlineStr">
+        <is>
+          <t>['F3']</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t xml:space="preserve"> 5 MAY 1980</t>
         </is>
@@ -882,34 +917,37 @@
           <t>I11</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" t="n">
+        <v>111</v>
+      </c>
+      <c r="D12" t="inlineStr">
         <is>
           <t xml:space="preserve"> Sarah /Watson/</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t xml:space="preserve"> 19 APR 1950</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="b">
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="b">
         <v>0</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>59</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>F5</t>
-        </is>
-      </c>
       <c r="J12" t="inlineStr">
+        <is>
+          <t>['F5']</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t xml:space="preserve"> 9 AUG 2009</t>
         </is>
@@ -926,7 +964,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -942,42 +980,47 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Husband ID</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Husband Name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Wife ID</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Wife Name</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>children</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>married</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>are divorced</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>divorced</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>are divorced</t>
         </is>
       </c>
     </row>
@@ -990,42 +1033,47 @@
           <t>F1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>122</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>I2</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Steven /Brindley/</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>I3</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Amy /Brooks/</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>['I1', 'I4']</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t xml:space="preserve"> 9 JUN 1992</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t xml:space="preserve"> 10 JUL 2015</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1036,38 +1084,43 @@
           <t>F2</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>133</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>I2</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t xml:space="preserve"> Steven /Brindley/</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>I7</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t xml:space="preserve"> Lisa /Rutherford/</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>['I8']</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t xml:space="preserve"> 12 JUL 2016</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1078,38 +1131,43 @@
           <t>F3</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>141</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>I9</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t xml:space="preserve"> Tim /Brindley/</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>I10</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t xml:space="preserve"> Selina /Rosemary/</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>['I2']</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t xml:space="preserve"> 3 APR 1967</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1120,40 +1178,43 @@
           <t>F4</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>158</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>I5</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t xml:space="preserve"> Erin /Brooks/</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>I6</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t xml:space="preserve"> Josie /Campbell/</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>['I3']</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t xml:space="preserve"> 7 APR 1967</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
       <c r="J5" t="b">
         <v>0</v>
       </c>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1164,34 +1225,39 @@
           <t>F5</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>151</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>I9</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t xml:space="preserve"> Tim /Brindley/</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>I11</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t xml:space="preserve"> Sarah /Watson/</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
         <is>
           <t xml:space="preserve"> 3 MAY 1985</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>